<commit_message>
fix: add missing SUM formula in `'VMMM questions'!G132`
</commit_message>
<xml_diff>
--- a/Maturity Assessment VMMM v2.xlsx
+++ b/Maturity Assessment VMMM v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ristoj/Downloads/Version-K01/Maturity Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raptor/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A1A427-7CD0-1B4C-9296-EA1315493155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24FCBD8-A0AC-DC49-8A50-A2534413DB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1020" windowWidth="33100" windowHeight="20580" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Maturity Level" sheetId="3" r:id="rId1"/>
@@ -805,9 +805,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -845,7 +845,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -951,7 +951,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1093,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1103,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D64A92-CB24-8346-8CE4-B27D7EACC050}">
   <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1539,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA35A465-1318-F645-901D-1F432B1ECEDB}">
   <dimension ref="A5:I159"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1548,7 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="107.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="2" customWidth="1"/>
-    <col min="5" max="8" width="11" hidden="1" customWidth="1"/>
+    <col min="5" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3942,6 +3942,10 @@
       </c>
       <c r="F132">
         <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <f>SUM(F132:F134)</f>
         <v>0</v>
       </c>
       <c r="H132" s="14">

</xml_diff>

<commit_message>
chore: hide columns E-H in `VMMM questions` sheet
</commit_message>
<xml_diff>
--- a/Maturity Assessment VMMM v2.xlsx
+++ b/Maturity Assessment VMMM v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raptor/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24FCBD8-A0AC-DC49-8A50-A2534413DB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C0A7EF-0D60-3D48-AE47-4E8DAA15A4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Maturity Level" sheetId="3" r:id="rId1"/>
@@ -1103,9 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D64A92-CB24-8346-8CE4-B27D7EACC050}">
   <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1539,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA35A465-1318-F645-901D-1F432B1ECEDB}">
   <dimension ref="A5:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1546,7 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="107.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="2" customWidth="1"/>
-    <col min="5" max="8" width="11" customWidth="1"/>
+    <col min="5" max="8" width="11" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add missing formula in `'VMMM questions'!G132` (#2)
* fix: add missing SUM formula in `'VMMM questions'!G132`

* chore: hide columns E-H in `VMMM questions` sheet
</commit_message>
<xml_diff>
--- a/Maturity Assessment VMMM v2.xlsx
+++ b/Maturity Assessment VMMM v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ristoj/Downloads/Version-K01/Maturity Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raptor/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A1A427-7CD0-1B4C-9296-EA1315493155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C0A7EF-0D60-3D48-AE47-4E8DAA15A4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1020" windowWidth="33100" windowHeight="20580" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{A8BD3F03-2723-9F4D-9FE2-CE71A9E80D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Maturity Level" sheetId="3" r:id="rId1"/>
@@ -805,9 +805,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -845,7 +845,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -951,7 +951,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1093,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1103,9 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D64A92-CB24-8346-8CE4-B27D7EACC050}">
   <dimension ref="B1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1540,7 +1538,7 @@
   <dimension ref="A5:I159"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -3942,6 +3940,10 @@
       </c>
       <c r="F132">
         <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <f>SUM(F132:F134)</f>
         <v>0</v>
       </c>
       <c r="H132" s="14">

</xml_diff>